<commit_message>
finished evaluation + documentation
</commit_message>
<xml_diff>
--- a/evalDataResultAnalysis.xlsx
+++ b/evalDataResultAnalysis.xlsx
@@ -8,19 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christianspiekermann/Uni/DataScienceTrumpTweets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC80969C-17B8-7F46-850C-39B30B892871}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24EDBBB6-97BD-A64D-8546-DB05E09A7889}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="114">
   <si>
     <t>id</t>
   </si>
@@ -28,15 +38,6 @@
     <t>content</t>
   </si>
   <si>
-    <t>Sentiment</t>
-  </si>
-  <si>
-    <t>blob</t>
-  </si>
-  <si>
-    <t>vader</t>
-  </si>
-  <si>
     <t>782698760514207744</t>
   </si>
   <si>
@@ -337,15 +338,6 @@
     <t>I am calling on Congress to send me a Bill that fully and permanently funds the LWCF and restores our National Parks. When I sign it into law, it will be HISTORIC for our beautiful public lands. ALL thanks to @ SenCoryGardner and @ SteveDaines, two GREAT Conservative Leaders!</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
     <t>n</t>
   </si>
   <si>
@@ -358,14 +350,35 @@
     <t>p</t>
   </si>
   <si>
-    <t>Senti1</t>
+    <t>TextBlob</t>
+  </si>
+  <si>
+    <t>VADER</t>
+  </si>
+  <si>
+    <t>Blob Korr</t>
+  </si>
+  <si>
+    <t>Vader Korr</t>
+  </si>
+  <si>
+    <t>Senti Pers1</t>
+  </si>
+  <si>
+    <t>Senti Pers2</t>
+  </si>
+  <si>
+    <t>Senti Pers3</t>
+  </si>
+  <si>
+    <t>Sent PersGes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -378,6 +391,20 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -387,7 +414,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -410,15 +437,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -721,18 +766,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="C11" zoomScale="110" workbookViewId="0">
+      <selection activeCell="J53" sqref="J53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="185.5" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" customWidth="1"/>
+    <col min="11" max="11" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -740,1016 +790,1798 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>106</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>107</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>30345</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
         <v>0.29599999999999999</v>
       </c>
+      <c r="F2" t="s">
+        <v>102</v>
+      </c>
       <c r="G2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="H2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2" t="s">
+        <v>102</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>26235</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>0.22500000000000001</v>
       </c>
       <c r="E3">
-        <v>0.22500000000000001</v>
-      </c>
-      <c r="F3">
         <v>0.61140000000000005</v>
       </c>
+      <c r="F3" t="s">
+        <v>102</v>
+      </c>
       <c r="G3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="H3" t="s">
+        <v>102</v>
+      </c>
+      <c r="I3" t="s">
+        <v>102</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>35387</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>0.75</v>
       </c>
       <c r="E4">
-        <v>0.75</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>105</v>
       </c>
       <c r="G4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="H4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I4" t="s">
+        <v>105</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>40676</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
         <v>0.31469999999999998</v>
       </c>
+      <c r="F5" t="s">
+        <v>102</v>
+      </c>
       <c r="G5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="H5" t="s">
+        <v>102</v>
+      </c>
+      <c r="I5" t="s">
+        <v>102</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>21606</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
         <v>0.38019999999999998</v>
       </c>
+      <c r="F6" t="s">
+        <v>105</v>
+      </c>
       <c r="G6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="H6" t="s">
+        <v>105</v>
+      </c>
+      <c r="I6" t="s">
+        <v>105</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>21778</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="D7">
+        <v>0.5</v>
       </c>
       <c r="E7">
-        <v>0.5</v>
-      </c>
-      <c r="F7">
         <v>0.31819999999999998</v>
       </c>
+      <c r="F7" t="s">
+        <v>105</v>
+      </c>
       <c r="G7" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="H7" t="s">
+        <v>105</v>
+      </c>
+      <c r="I7" t="s">
+        <v>105</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>25418</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8">
-        <v>0</v>
+      <c r="F8" t="s">
+        <v>104</v>
       </c>
       <c r="G8" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+      <c r="H8" t="s">
+        <v>104</v>
+      </c>
+      <c r="I8" t="s">
+        <v>104</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>21876</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="D9">
+        <v>0.72499999999999998</v>
       </c>
       <c r="E9">
-        <v>0.72499999999999998</v>
-      </c>
-      <c r="F9">
         <v>0.84809999999999997</v>
       </c>
+      <c r="F9" t="s">
+        <v>102</v>
+      </c>
       <c r="G9" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" t="s">
+        <v>105</v>
+      </c>
+      <c r="I9" t="s">
+        <v>105</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>36219</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>19</v>
+      </c>
+      <c r="D10">
+        <v>0.46666666666666667</v>
       </c>
       <c r="E10">
-        <v>0.46666666666666667</v>
-      </c>
-      <c r="F10">
         <v>0.57069999999999999</v>
       </c>
+      <c r="F10" t="s">
+        <v>102</v>
+      </c>
       <c r="G10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="H10" t="s">
+        <v>104</v>
+      </c>
+      <c r="I10" t="s">
+        <v>102</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>13826</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="D11">
+        <v>0.26666666666666672</v>
       </c>
       <c r="E11">
-        <v>0.26666666666666672</v>
-      </c>
-      <c r="F11">
         <v>0.89729999999999999</v>
       </c>
+      <c r="F11" t="s">
+        <v>105</v>
+      </c>
       <c r="G11" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="H11" t="s">
+        <v>105</v>
+      </c>
+      <c r="I11" t="s">
+        <v>105</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>16296</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>23</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
-      <c r="F12">
-        <v>0</v>
+      <c r="F12" t="s">
+        <v>102</v>
       </c>
       <c r="G12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="H12" t="s">
+        <v>102</v>
+      </c>
+      <c r="I12" t="s">
+        <v>102</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>10144</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>25</v>
+      </c>
+      <c r="D13">
+        <v>0.35</v>
       </c>
       <c r="E13">
-        <v>0.35</v>
-      </c>
-      <c r="F13">
         <v>0.4501</v>
       </c>
+      <c r="F13" t="s">
+        <v>102</v>
+      </c>
       <c r="G13" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="H13" t="s">
+        <v>102</v>
+      </c>
+      <c r="I13" t="s">
+        <v>102</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>31501</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
         <v>0.49390000000000001</v>
       </c>
+      <c r="F14" t="s">
+        <v>105</v>
+      </c>
       <c r="G14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="H14" t="s">
+        <v>104</v>
+      </c>
+      <c r="I14" t="s">
+        <v>105</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>34694</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>29</v>
+      </c>
+      <c r="D15">
+        <v>0.22348484848484851</v>
       </c>
       <c r="E15">
-        <v>0.22348484848484851</v>
-      </c>
-      <c r="F15">
         <v>0.66210000000000002</v>
       </c>
+      <c r="F15" t="s">
+        <v>102</v>
+      </c>
       <c r="G15" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="H15" t="s">
+        <v>102</v>
+      </c>
+      <c r="I15" t="s">
+        <v>102</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>18834</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>31</v>
+      </c>
+      <c r="D16">
+        <v>0.90625</v>
       </c>
       <c r="E16">
-        <v>0.90625</v>
-      </c>
-      <c r="F16">
         <v>0.82640000000000002</v>
       </c>
+      <c r="F16" t="s">
+        <v>103</v>
+      </c>
       <c r="G16" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="H16" t="s">
+        <v>105</v>
+      </c>
+      <c r="I16" t="s">
+        <v>105</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>21535</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="D17">
+        <v>0.25</v>
       </c>
       <c r="E17">
-        <v>0.25</v>
-      </c>
-      <c r="F17">
         <v>7.7200000000000005E-2</v>
       </c>
+      <c r="F17" t="s">
+        <v>105</v>
+      </c>
       <c r="G17" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="H17" t="s">
+        <v>104</v>
+      </c>
+      <c r="I17" t="s">
+        <v>105</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>41678</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>35</v>
+      </c>
+      <c r="D18">
+        <v>-0.20940170940170941</v>
       </c>
       <c r="E18">
-        <v>-0.20940170940170941</v>
-      </c>
-      <c r="F18">
         <v>0.17030000000000001</v>
       </c>
+      <c r="F18" t="s">
+        <v>102</v>
+      </c>
       <c r="G18" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="H18" t="s">
+        <v>102</v>
+      </c>
+      <c r="I18" t="s">
+        <v>102</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>2971</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>37</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
         <v>-0.61240000000000006</v>
       </c>
+      <c r="F19" t="s">
+        <v>102</v>
+      </c>
       <c r="G19" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="H19" t="s">
+        <v>102</v>
+      </c>
+      <c r="I19" t="s">
+        <v>102</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>17963</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>39</v>
+      </c>
+      <c r="D20">
+        <v>0.26666666666666672</v>
       </c>
       <c r="E20">
-        <v>0.26666666666666672</v>
-      </c>
-      <c r="F20">
         <v>0.2235</v>
       </c>
+      <c r="F20" t="s">
+        <v>102</v>
+      </c>
       <c r="G20" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="H20" t="s">
+        <v>102</v>
+      </c>
+      <c r="I20" t="s">
+        <v>102</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>33345</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>41</v>
+      </c>
+      <c r="D21">
+        <v>-7.3842592592592599E-2</v>
       </c>
       <c r="E21">
-        <v>-7.3842592592592599E-2</v>
-      </c>
-      <c r="F21">
         <v>-0.31230000000000002</v>
       </c>
+      <c r="F21" t="s">
+        <v>102</v>
+      </c>
       <c r="G21" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="H21" t="s">
+        <v>102</v>
+      </c>
+      <c r="I21" t="s">
+        <v>102</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>22253</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>43</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
       </c>
       <c r="E22">
         <v>0</v>
       </c>
-      <c r="F22">
-        <v>0</v>
+      <c r="F22" t="s">
+        <v>104</v>
       </c>
       <c r="G22" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+      <c r="H22" t="s">
+        <v>104</v>
+      </c>
+      <c r="I22" t="s">
+        <v>104</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22232</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C23" t="s">
-        <v>48</v>
+        <v>45</v>
+      </c>
+      <c r="D23">
+        <v>4.5454545454545449E-2</v>
       </c>
       <c r="E23">
-        <v>4.5454545454545449E-2</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>105</v>
       </c>
       <c r="G23" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+      <c r="H23" t="s">
+        <v>104</v>
+      </c>
+      <c r="I23" t="s">
+        <v>104</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>29910</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>47</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
       </c>
       <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
         <v>0.4738</v>
       </c>
+      <c r="F24" t="s">
+        <v>105</v>
+      </c>
       <c r="G24" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="H24" t="s">
+        <v>105</v>
+      </c>
+      <c r="I24" t="s">
+        <v>105</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>31308</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
+        <v>49</v>
+      </c>
+      <c r="D25">
+        <v>0.1825</v>
       </c>
       <c r="E25">
-        <v>0.1825</v>
-      </c>
-      <c r="F25">
         <v>-8.6800000000000002E-2</v>
       </c>
+      <c r="F25" t="s">
+        <v>105</v>
+      </c>
       <c r="G25" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="H25" t="s">
+        <v>105</v>
+      </c>
+      <c r="I25" t="s">
+        <v>105</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>13332</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C26" t="s">
-        <v>54</v>
+        <v>51</v>
+      </c>
+      <c r="D26">
+        <v>0.625</v>
       </c>
       <c r="E26">
-        <v>0.625</v>
-      </c>
-      <c r="F26">
         <v>0.38019999999999998</v>
       </c>
+      <c r="F26" t="s">
+        <v>104</v>
+      </c>
       <c r="G26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="H26" t="s">
+        <v>105</v>
+      </c>
+      <c r="I26" t="s">
+        <v>105</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>5085</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C27" t="s">
-        <v>56</v>
+        <v>53</v>
+      </c>
+      <c r="D27">
+        <v>-3.1818181818181829E-2</v>
       </c>
       <c r="E27">
-        <v>-3.1818181818181829E-2</v>
-      </c>
-      <c r="F27">
         <v>-0.81759999999999999</v>
       </c>
+      <c r="F27" t="s">
+        <v>102</v>
+      </c>
       <c r="G27" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="H27" t="s">
+        <v>102</v>
+      </c>
+      <c r="I27" t="s">
+        <v>102</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>21376</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C28" t="s">
-        <v>58</v>
+        <v>55</v>
+      </c>
+      <c r="D28">
+        <v>-0.4</v>
       </c>
       <c r="E28">
-        <v>-0.4</v>
-      </c>
-      <c r="F28">
         <v>-0.57330000000000003</v>
       </c>
+      <c r="F28" t="s">
+        <v>104</v>
+      </c>
       <c r="G28" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="H28" t="s">
+        <v>102</v>
+      </c>
+      <c r="I28" t="s">
+        <v>102</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>19224</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
+        <v>57</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
       </c>
       <c r="E29">
         <v>0</v>
       </c>
-      <c r="F29">
-        <v>0</v>
+      <c r="F29" t="s">
+        <v>104</v>
       </c>
       <c r="G29" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+      <c r="H29" t="s">
+        <v>104</v>
+      </c>
+      <c r="I29" t="s">
+        <v>104</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>31042</v>
       </c>
       <c r="B30" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C30" t="s">
-        <v>62</v>
+        <v>59</v>
+      </c>
+      <c r="D30">
+        <v>-7.4999999999999997E-2</v>
       </c>
       <c r="E30">
-        <v>-7.4999999999999997E-2</v>
-      </c>
-      <c r="F30">
         <v>0.42149999999999999</v>
       </c>
+      <c r="F30" t="s">
+        <v>102</v>
+      </c>
       <c r="G30" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="H30" t="s">
+        <v>102</v>
+      </c>
+      <c r="I30" t="s">
+        <v>102</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>41022</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C31" t="s">
-        <v>64</v>
+        <v>61</v>
+      </c>
+      <c r="D31">
+        <v>0.125</v>
       </c>
       <c r="E31">
-        <v>0.125</v>
-      </c>
-      <c r="F31">
         <v>0.31819999999999998</v>
       </c>
+      <c r="F31" t="s">
+        <v>102</v>
+      </c>
       <c r="G31" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="H31" t="s">
+        <v>102</v>
+      </c>
+      <c r="I31" t="s">
+        <v>102</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>26568</v>
       </c>
       <c r="B32" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C32" t="s">
-        <v>66</v>
+        <v>63</v>
+      </c>
+      <c r="D32">
+        <v>0.5</v>
       </c>
       <c r="E32">
-        <v>0.5</v>
-      </c>
-      <c r="F32">
         <v>0.5232</v>
       </c>
+      <c r="F32" t="s">
+        <v>102</v>
+      </c>
       <c r="G32" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+      <c r="H32" t="s">
+        <v>104</v>
+      </c>
+      <c r="I32" t="s">
+        <v>104</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>27153</v>
       </c>
       <c r="B33" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C33" t="s">
-        <v>68</v>
+        <v>65</v>
+      </c>
+      <c r="D33">
+        <v>0.15625</v>
       </c>
       <c r="E33">
-        <v>0.15625</v>
-      </c>
-      <c r="F33">
         <v>-0.83489999999999998</v>
       </c>
+      <c r="F33" t="s">
+        <v>102</v>
+      </c>
       <c r="G33" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="H33" t="s">
+        <v>102</v>
+      </c>
+      <c r="I33" t="s">
+        <v>102</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>28688</v>
       </c>
       <c r="B34" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C34" t="s">
-        <v>70</v>
+        <v>67</v>
+      </c>
+      <c r="D34">
+        <v>6.8181818181818177E-2</v>
       </c>
       <c r="E34">
-        <v>6.8181818181818177E-2</v>
-      </c>
-      <c r="F34">
         <v>0.62390000000000001</v>
       </c>
+      <c r="F34" t="s">
+        <v>104</v>
+      </c>
       <c r="G34" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="H34" t="s">
+        <v>105</v>
+      </c>
+      <c r="I34" t="s">
+        <v>105</v>
+      </c>
+      <c r="J34">
+        <v>1</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>18264</v>
       </c>
       <c r="B35" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C35" t="s">
-        <v>72</v>
+        <v>69</v>
+      </c>
+      <c r="D35">
+        <v>0.7</v>
       </c>
       <c r="E35">
-        <v>0.7</v>
-      </c>
-      <c r="F35">
         <v>0.624</v>
       </c>
+      <c r="F35" t="s">
+        <v>105</v>
+      </c>
       <c r="G35" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="H35" t="s">
+        <v>105</v>
+      </c>
+      <c r="I35" t="s">
+        <v>105</v>
+      </c>
+      <c r="J35">
+        <v>1</v>
+      </c>
+      <c r="K35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>16226</v>
       </c>
       <c r="B36" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C36" t="s">
-        <v>74</v>
+        <v>71</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
       </c>
       <c r="E36">
-        <v>0</v>
-      </c>
-      <c r="F36">
         <v>0.91</v>
       </c>
+      <c r="F36" t="s">
+        <v>105</v>
+      </c>
       <c r="G36" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="H36" t="s">
+        <v>105</v>
+      </c>
+      <c r="I36" t="s">
+        <v>105</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>25109</v>
       </c>
       <c r="B37" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C37" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
       </c>
       <c r="E37">
         <v>0</v>
       </c>
-      <c r="F37">
-        <v>0</v>
+      <c r="F37" t="s">
+        <v>103</v>
       </c>
       <c r="G37" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+      <c r="H37" t="s">
+        <v>104</v>
+      </c>
+      <c r="I37" t="s">
+        <v>104</v>
+      </c>
+      <c r="J37">
+        <v>1</v>
+      </c>
+      <c r="K37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>13820</v>
       </c>
       <c r="B38" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C38" t="s">
-        <v>78</v>
+        <v>75</v>
+      </c>
+      <c r="D38">
+        <v>0.625</v>
       </c>
       <c r="E38">
-        <v>0.625</v>
-      </c>
-      <c r="F38">
         <v>-0.52549999999999997</v>
       </c>
+      <c r="F38" t="s">
+        <v>104</v>
+      </c>
       <c r="G38" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="H38" t="s">
+        <v>102</v>
+      </c>
+      <c r="I38" t="s">
+        <v>102</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>35895</v>
       </c>
       <c r="B39" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C39" t="s">
-        <v>80</v>
+        <v>77</v>
+      </c>
+      <c r="D39">
+        <v>0.3</v>
       </c>
       <c r="E39">
-        <v>0.3</v>
-      </c>
-      <c r="F39">
         <v>0.57189999999999996</v>
       </c>
+      <c r="F39" t="s">
+        <v>105</v>
+      </c>
       <c r="G39" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="H39" t="s">
+        <v>104</v>
+      </c>
+      <c r="I39" t="s">
+        <v>105</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+      <c r="K39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>30499</v>
       </c>
       <c r="B40" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C40" t="s">
-        <v>82</v>
+        <v>79</v>
+      </c>
+      <c r="D40">
+        <v>0.125</v>
       </c>
       <c r="E40">
-        <v>0.125</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="F40" t="s">
+        <v>102</v>
       </c>
       <c r="G40" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+      <c r="H40" t="s">
+        <v>104</v>
+      </c>
+      <c r="I40" t="s">
+        <v>104</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>34355</v>
       </c>
       <c r="B41" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C41" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="D41">
+        <v>0.20699999999999999</v>
       </c>
       <c r="E41">
-        <v>0.20699999999999999</v>
-      </c>
-      <c r="F41">
         <v>0.64759999999999995</v>
       </c>
+      <c r="F41" t="s">
+        <v>102</v>
+      </c>
       <c r="G41" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="H41" t="s">
+        <v>102</v>
+      </c>
+      <c r="I41" t="s">
+        <v>102</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>331</v>
       </c>
       <c r="B42" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C42" t="s">
-        <v>86</v>
+        <v>83</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
       </c>
       <c r="E42">
-        <v>0</v>
-      </c>
-      <c r="F42">
         <v>-0.82530000000000003</v>
       </c>
+      <c r="F42" t="s">
+        <v>102</v>
+      </c>
       <c r="G42" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="H42" t="s">
+        <v>102</v>
+      </c>
+      <c r="I42" t="s">
+        <v>102</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>2786</v>
       </c>
       <c r="B43" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C43" t="s">
-        <v>88</v>
+        <v>85</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
       </c>
       <c r="E43">
-        <v>0</v>
-      </c>
-      <c r="F43">
         <v>-0.29599999999999999</v>
       </c>
+      <c r="F43" t="s">
+        <v>102</v>
+      </c>
       <c r="G43" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="H43" t="s">
+        <v>102</v>
+      </c>
+      <c r="I43" t="s">
+        <v>102</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>7592</v>
       </c>
       <c r="B44" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C44" t="s">
-        <v>90</v>
+        <v>87</v>
+      </c>
+      <c r="D44">
+        <v>-0.79999999999999993</v>
       </c>
       <c r="E44">
-        <v>-0.79999999999999993</v>
-      </c>
-      <c r="F44">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="F44" t="s">
+        <v>102</v>
       </c>
       <c r="G44" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="H44" t="s">
+        <v>102</v>
+      </c>
+      <c r="I44" t="s">
+        <v>102</v>
+      </c>
+      <c r="J44">
+        <v>1</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>8265</v>
       </c>
       <c r="B45" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C45" t="s">
-        <v>92</v>
+        <v>89</v>
+      </c>
+      <c r="D45">
+        <v>-1</v>
       </c>
       <c r="E45">
-        <v>-1</v>
-      </c>
-      <c r="F45">
         <v>-0.60160000000000002</v>
       </c>
+      <c r="F45" t="s">
+        <v>104</v>
+      </c>
       <c r="G45" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="H45" t="s">
+        <v>105</v>
+      </c>
+      <c r="I45" t="s">
+        <v>103</v>
+      </c>
+      <c r="J45" t="s">
+        <v>103</v>
+      </c>
+      <c r="K45" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>20330</v>
       </c>
       <c r="B46" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C46" t="s">
-        <v>94</v>
+        <v>91</v>
+      </c>
+      <c r="D46">
+        <v>0.05</v>
       </c>
       <c r="E46">
-        <v>0.05</v>
-      </c>
-      <c r="F46">
         <v>-0.2732</v>
       </c>
+      <c r="F46" t="s">
+        <v>104</v>
+      </c>
       <c r="G46" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="H46" t="s">
+        <v>105</v>
+      </c>
+      <c r="I46" t="s">
+        <v>105</v>
+      </c>
+      <c r="J46">
+        <v>1</v>
+      </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>41786</v>
       </c>
       <c r="B47" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C47" t="s">
-        <v>96</v>
+        <v>93</v>
+      </c>
+      <c r="D47">
+        <v>-5.0000000000000017E-2</v>
       </c>
       <c r="E47">
-        <v>-5.0000000000000017E-2</v>
-      </c>
-      <c r="F47">
         <v>-0.52549999999999997</v>
       </c>
+      <c r="F47" t="s">
+        <v>102</v>
+      </c>
       <c r="G47" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="H47" t="s">
+        <v>102</v>
+      </c>
+      <c r="I47" t="s">
+        <v>102</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+      <c r="K47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>17130</v>
       </c>
       <c r="B48" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C48" t="s">
-        <v>98</v>
+        <v>95</v>
+      </c>
+      <c r="D48">
+        <v>-9.9999999999999992E-2</v>
       </c>
       <c r="E48">
-        <v>-9.9999999999999992E-2</v>
-      </c>
-      <c r="F48">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="F48" t="s">
+        <v>104</v>
       </c>
       <c r="G48" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+      <c r="H48" t="s">
+        <v>104</v>
+      </c>
+      <c r="I48" t="s">
+        <v>104</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>22956</v>
       </c>
       <c r="B49" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C49" t="s">
-        <v>100</v>
+        <v>97</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
       </c>
       <c r="E49">
-        <v>0</v>
-      </c>
-      <c r="F49">
         <v>0.128</v>
       </c>
+      <c r="F49" t="s">
+        <v>104</v>
+      </c>
       <c r="G49" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="H49" t="s">
+        <v>104</v>
+      </c>
+      <c r="I49" t="s">
+        <v>104</v>
+      </c>
+      <c r="J49">
+        <v>1</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>24492</v>
       </c>
       <c r="B50" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C50" t="s">
-        <v>102</v>
+        <v>99</v>
+      </c>
+      <c r="D50">
+        <v>8.8942307692307709E-2</v>
       </c>
       <c r="E50">
-        <v>8.8942307692307709E-2</v>
-      </c>
-      <c r="F50">
         <v>0.30990000000000001</v>
       </c>
+      <c r="F50" t="s">
+        <v>105</v>
+      </c>
       <c r="G50" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="H50" t="s">
+        <v>102</v>
+      </c>
+      <c r="I50" t="s">
+        <v>105</v>
+      </c>
+      <c r="J50">
+        <v>1</v>
+      </c>
+      <c r="K50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>41751</v>
       </c>
       <c r="B51" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C51" t="s">
-        <v>104</v>
+        <v>101</v>
+      </c>
+      <c r="D51">
+        <v>0.41</v>
       </c>
       <c r="E51">
-        <v>0.41</v>
-      </c>
-      <c r="F51">
         <v>0.93400000000000005</v>
       </c>
+      <c r="F51" t="s">
+        <v>105</v>
+      </c>
       <c r="G51" t="s">
-        <v>111</v>
+        <v>105</v>
+      </c>
+      <c r="H51" t="s">
+        <v>105</v>
+      </c>
+      <c r="I51" t="s">
+        <v>105</v>
+      </c>
+      <c r="J51">
+        <v>1</v>
+      </c>
+      <c r="K51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J52" s="4">
+        <f>SUM(J2:J51)</f>
+        <v>26</v>
+      </c>
+      <c r="K52" s="4">
+        <f>SUM(K2:K51)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J53" s="4">
+        <f>J52/49</f>
+        <v>0.53061224489795922</v>
+      </c>
+      <c r="K53" s="4">
+        <f>K52/49</f>
+        <v>0.63265306122448983</v>
       </c>
     </row>
   </sheetData>

</xml_diff>